<commit_message>
Deactivate the new MODIS pextra table 126 variables in default situation, put them on the identified missing list #746. This fixes the default test-all case. When pextra is switched on th evraiables will be included as it should.
</commit_message>
<xml_diff>
--- a/ece2cmor3/resources/list-of-identified-missing-cmip6-requested-variables.xlsx
+++ b/ece2cmor3/resources/list-of-identified-missing-cmip6-requested-variables.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="252">
   <si>
     <t xml:space="preserve">Table</t>
   </si>
@@ -817,6 +817,24 @@
   <si>
     <t xml:space="preserve">CF3hr</t>
   </si>
+  <si>
+    <t xml:space="preserve">cltmodis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implemented in EC-Earth table 126: grib code 47.126</t>
+  </si>
+  <si>
+    <t xml:space="preserve">clwmodis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implemented in EC-Earth table 126: grib code 48.126</t>
+  </si>
+  <si>
+    <t xml:space="preserve">climodis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implemented in EC-Earth table 126: grib code 49.126</t>
+  </si>
 </sst>
 </file>
 
@@ -825,7 +843,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -862,6 +880,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -906,7 +930,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -919,14 +943,18 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -992,17 +1020,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:K1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A32" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A58" activeCellId="0" sqref="A58"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A65" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A94" activeCellId="0" sqref="92:94"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.71"/>
@@ -1013,9 +1041,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="4.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="80.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="15.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="200.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="200.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="80.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3068,6 +3095,48 @@
       </c>
       <c r="I85" s="0" t="s">
         <v>192</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="B92" s="0" t="s">
+        <v>246</v>
+      </c>
+      <c r="C92" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H92" s="0" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="B93" s="0" t="s">
+        <v>248</v>
+      </c>
+      <c r="C93" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H93" s="3" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="B94" s="0" t="s">
+        <v>250</v>
+      </c>
+      <c r="C94" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H94" s="3" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -3083,8 +3152,8 @@
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
Deactivate reffclis (24.126) from default situation #760, added to the identified missing list #746. This fixes the default test-all case. When pextra is switched on th evraiables will be included as it should.
</commit_message>
<xml_diff>
--- a/ece2cmor3/resources/list-of-identified-missing-cmip6-requested-variables.xlsx
+++ b/ece2cmor3/resources/list-of-identified-missing-cmip6-requested-variables.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="254">
   <si>
     <t xml:space="preserve">Table</t>
   </si>
@@ -834,6 +834,12 @@
   </si>
   <si>
     <t xml:space="preserve">Implemented in EC-Earth table 126: grib code 49.126</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reffclis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implemented in EC-Earth table 126: grib code 24.126</t>
   </si>
 </sst>
 </file>
@@ -930,7 +936,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -941,6 +947,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -1027,10 +1037,10 @@
   <dimension ref="A1:K1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A65" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A94" activeCellId="0" sqref="92:94"/>
+      <selection pane="topLeft" activeCell="A98" activeCellId="0" sqref="A98"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.71"/>
@@ -3137,6 +3147,28 @@
       </c>
       <c r="H94" s="3" t="s">
         <v>251</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="B96" s="0" t="s">
+        <v>252</v>
+      </c>
+      <c r="H96" s="4" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="0" t="s">
+        <v>245</v>
+      </c>
+      <c r="B97" s="0" t="s">
+        <v>252</v>
+      </c>
+      <c r="H97" s="4" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>